<commit_message>
se agrega columna de especificacion funcional a la estrategia
</commit_message>
<xml_diff>
--- a/Conceptos Avanzados Ingenieria Software/TSP/Ciclo I/Strat/Diseño Conceptual.xlsx
+++ b/Conceptos Avanzados Ingenieria Software/TSP/Ciclo I/Strat/Diseño Conceptual.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Assembly</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>EF</t>
   </si>
 </sst>
 </file>
@@ -628,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +642,7 @@
     <col min="1" max="1" width="132" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -647,7 +650,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
@@ -657,7 +660,7 @@
       </c>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,8 +676,11 @@
       <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -695,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -711,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -727,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -744,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -760,7 +766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -781,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -797,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -813,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -829,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Actualización Workbook Semana 4
</commit_message>
<xml_diff>
--- a/Conceptos Avanzados Ingenieria Software/TSP/Ciclo I/Strat/Diseño Conceptual.xlsx
+++ b/Conceptos Avanzados Ingenieria Software/TSP/Ciclo I/Strat/Diseño Conceptual.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="19875" windowHeight="7650"/>
+    <workbookView xWindow="480" yWindow="420" windowWidth="19416" windowHeight="7656"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$12:$B$21</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>Lector Archivos</t>
-  </si>
-  <si>
-    <t>LOS/HORA</t>
   </si>
   <si>
     <t>Identificar archivos a comparar en cada versión (versión previa del archivo)</t>
@@ -123,9 +120,6 @@
     <t>Escribir modificaciones (Etiquetas)</t>
   </si>
   <si>
-    <t>Crear una etiqueta de referencia para cada línea agrega o borrada para indicar el número del cambio</t>
-  </si>
-  <si>
     <t>Proveer una etiqueta de cambio en el comentario del encabezado del programa o clase, que indique el número del cambio, la fecha del cambio, quién hizo el cambio, porqué lo hizo, y el LOC total adicionado y borrado</t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>Para programas nuevos contar el programa y agregar las etiquetas con versión 0</t>
   </si>
   <si>
-    <t>En la etiqueta del programa indicar las líneas agregas, borradas y totales de todo el programa</t>
-  </si>
-  <si>
     <t>Enumerar cada línea agregada y borrada en comentarios a la derecha de la línea</t>
   </si>
   <si>
@@ -165,9 +156,6 @@
     <t>Agregar números de líneas</t>
   </si>
   <si>
-    <t>para líneas muy grandes pasar a la siguiente línea</t>
-  </si>
-  <si>
     <t>Mantener la indentación original</t>
   </si>
   <si>
@@ -204,20 +192,32 @@
     <t>El programa debe funcionar inicialmente para JAVA.</t>
   </si>
   <si>
-    <t>Crear fabricas para permitir el funcionamiento en diversos lenguajes</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>EF</t>
+  </si>
+  <si>
+    <t>LOCS/HORA</t>
+  </si>
+  <si>
+    <t>Crear una etiqueta de referencia para cada línea agregada o borrada para indicar el número del cambio</t>
+  </si>
+  <si>
+    <t>En la etiqueta del programa indicar las líneas agregadas, borradas y totales de todo el programa</t>
+  </si>
+  <si>
+    <t>Para líneas muy grandes pasar a la siguiente línea</t>
+  </si>
+  <si>
+    <t>Crear fábricas para permitir el funcionamiento en diversos lenguajes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,7 +345,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -419,7 +419,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -454,7 +453,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -630,29 +628,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="132" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="B1" s="6">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
@@ -660,27 +658,27 @@
       </c>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -701,9 +699,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>30</v>
@@ -717,9 +715,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -733,9 +731,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
         <f>SUM(B10)</f>
@@ -750,9 +748,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -766,9 +764,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2">
         <f>SUM(B13:B21)</f>
@@ -787,9 +785,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -803,9 +801,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>15</v>
@@ -819,9 +817,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -835,9 +833,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>120</v>
@@ -851,18 +849,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>50</v>
@@ -876,14 +874,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="B20">
         <v>30</v>
@@ -897,18 +895,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2">
         <f>SUM(B24:B40)</f>
@@ -927,18 +925,18 @@
         <v>24.074074074074073</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25">
         <v>50</v>
@@ -952,9 +950,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>150</v>
@@ -968,9 +966,9 @@
         <v>5.5555555555555554</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27">
         <v>150</v>
@@ -984,9 +982,9 @@
         <v>5.5555555555555554</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C28">
         <v>90</v>
@@ -1000,18 +998,18 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30">
         <v>50</v>
@@ -1025,27 +1023,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C33">
         <v>50</v>
@@ -1055,9 +1053,9 @@
         <v>1.8518518518518519</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C34">
         <v>60</v>
@@ -1067,9 +1065,9 @@
         <v>2.2222222222222223</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C35">
         <v>50</v>
@@ -1079,9 +1077,9 @@
         <v>1.8518518518518519</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C36">
         <v>100</v>
@@ -1091,45 +1089,45 @@
         <v>3.7037037037037037</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="4" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B42" s="2">
         <f>SUM(B43:B45)</f>
@@ -1148,9 +1146,9 @@
         <v>12.962962962962962</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C43">
         <v>250</v>
@@ -1164,9 +1162,9 @@
         <v>9.2592592592592595</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C44">
         <v>50</v>
@@ -1180,9 +1178,9 @@
         <v>1.8518518518518519</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C45">
         <v>50</v>
@@ -1196,9 +1194,9 @@
         <v>1.8518518518518519</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B47" s="2">
         <f>SUM(B48:B50)</f>
@@ -1217,36 +1215,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B52" s="2">
         <f>SUM(B53:B54)</f>
@@ -1265,9 +1263,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>40</v>
@@ -1277,9 +1275,9 @@
         <v>1.4814814814814814</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B54">
         <v>80</v>
@@ -1289,9 +1287,9 @@
         <v>2.9629629629629628</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B56">
         <f>B52+B47+B42+B23+B12+B9+B5</f>
@@ -1321,24 +1319,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>